<commit_message>
Adding creative flow_matching.py for Dani's part 3 of the final
</commit_message>
<xml_diff>
--- a/Averages.xlsx
+++ b/Averages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danipeterson/Documents/UVU/Fall2025/Algorithms/Final/Analysis-of-Algorithms-Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889555EB-8E41-AF49-97B9-5AABCCA17FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C22D25A-980D-7F46-B4DB-FE05F3EDD048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" xr2:uid="{57B453D2-AB82-F748-BE03-9A48BBCB7B75}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J6"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>